<commit_message>
modified test for special cases in menopause and age_fup
</commit_message>
<xml_diff>
--- a/data/DATA_CARLA_P2.xlsx
+++ b/data/DATA_CARLA_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A86028-6075-43A3-B834-6949A4F35E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480E8DD7-023D-4153-A753-7E30FD1E3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9066751A-66DC-4340-90DF-5664720171E7}"/>
   </bookViews>
@@ -195,6 +195,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,9 +227,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -563,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE73C3D-BCFB-4A74-BF42-1DB204207ABB}">
   <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -734,7 +739,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>118.994184367439</v>
       </c>
       <c r="E2">
@@ -770,6 +775,9 @@
       <c r="Q2">
         <v>1</v>
       </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
       <c r="S2">
         <v>1</v>
       </c>
@@ -819,7 +827,7 @@
         <v>30456</v>
       </c>
       <c r="AL2" s="1">
-        <v>36757</v>
+        <v>35296</v>
       </c>
       <c r="AM2" s="1">
         <v>39345</v>
@@ -868,7 +876,7 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>78.994400954538307</v>
       </c>
       <c r="E3">
@@ -905,10 +913,7 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
         <v>82</v>
@@ -952,9 +957,7 @@
       <c r="AL3" s="1">
         <v>36758</v>
       </c>
-      <c r="AM3" s="1">
-        <v>39346</v>
-      </c>
+      <c r="AM3" s="1"/>
       <c r="AN3">
         <v>102.363734717235</v>
       </c>
@@ -996,7 +999,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>100.25163857327</v>
       </c>
       <c r="E4">
@@ -1027,10 +1030,7 @@
         <v>73.538527165800801</v>
       </c>
       <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>9</v>
@@ -1124,8 +1124,8 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5">
-        <v>116.909199293269</v>
+      <c r="D5" s="3">
+        <v>44.999000000000002</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1206,11 +1206,9 @@
         <v>30459</v>
       </c>
       <c r="AL5" s="1">
-        <v>36760</v>
-      </c>
-      <c r="AM5" s="1">
-        <v>39348</v>
-      </c>
+        <v>38221</v>
+      </c>
+      <c r="AM5" s="1"/>
       <c r="AN5">
         <v>112.16938545940199</v>
       </c>
@@ -1252,8 +1250,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>77.337107984122795</v>
+      <c r="D6" s="2">
+        <v>45</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1280,9 +1278,6 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>2</v>
-      </c>
-      <c r="R6">
         <v>2</v>
       </c>
       <c r="S6">
@@ -1383,8 +1378,8 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>70.170231586687393</v>
+      <c r="D7" s="2">
+        <v>55.01</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1410,8 +1405,8 @@
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="R7">
-        <v>3</v>
+      <c r="Q7">
+        <v>2</v>
       </c>
       <c r="S7">
         <v>9</v>
@@ -1465,7 +1460,7 @@
         <v>30461</v>
       </c>
       <c r="AL7" s="1">
-        <v>36762</v>
+        <v>36769</v>
       </c>
       <c r="AM7" s="1">
         <v>39350</v>
@@ -1506,5 +1501,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>